<commit_message>
chore: trigger clean build and ignore temp files
</commit_message>
<xml_diff>
--- a/Akun_Fasilitator_Kokulikuler.xlsx
+++ b/Akun_Fasilitator_Kokulikuler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aplikasi Web AI\LP Kokulikuler SMAN 1 Belitang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90FC69C-6490-4EEA-B79F-60431C6429A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348856A3-8BA8-4D8D-839D-474ECD4D62EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1038,12 +1038,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="30.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update: harmonize program title and add 'dan Kekinian' branding
</commit_message>
<xml_diff>
--- a/Akun_Fasilitator_Kokulikuler.xlsx
+++ b/Akun_Fasilitator_Kokulikuler.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aplikasi Web AI\LP Kokulikuler SMAN 1 Belitang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348856A3-8BA8-4D8D-839D-474ECD4D62EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB5E5A9-8D36-4E33-A4FA-9F7D05114F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$3:$3</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="220">
   <si>
     <t>No</t>
   </si>
@@ -40,9 +43,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>X. 1</t>
-  </si>
-  <si>
     <t>Sukirno, S.Pd.</t>
   </si>
   <si>
@@ -64,9 +64,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>X. 2</t>
-  </si>
-  <si>
     <t>Handaroh, S.Pd.</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>X. 3</t>
-  </si>
-  <si>
     <t>Flortentinus Supriyanto, S.Pd.</t>
   </si>
   <si>
@@ -106,9 +100,6 @@
     <t>7</t>
   </si>
   <si>
-    <t>X. 4</t>
-  </si>
-  <si>
     <t>Siti Anita, S.Pd.</t>
   </si>
   <si>
@@ -127,9 +118,6 @@
     <t>9</t>
   </si>
   <si>
-    <t>X. 5</t>
-  </si>
-  <si>
     <t>Atik Setianingsih, S.Pd.</t>
   </si>
   <si>
@@ -148,9 +136,6 @@
     <t>11</t>
   </si>
   <si>
-    <t>X. 6</t>
-  </si>
-  <si>
     <t>Wiwik Eko Prihatin, S.Pd., M.M.</t>
   </si>
   <si>
@@ -169,9 +154,6 @@
     <t>13</t>
   </si>
   <si>
-    <t>X. 7</t>
-  </si>
-  <si>
     <t>Azuari Dian Prasasti, S.Pd.</t>
   </si>
   <si>
@@ -190,9 +172,6 @@
     <t>15</t>
   </si>
   <si>
-    <t>X. 8</t>
-  </si>
-  <si>
     <t>Fajar Abdul Majid, S.Pd</t>
   </si>
   <si>
@@ -211,9 +190,6 @@
     <t>17</t>
   </si>
   <si>
-    <t>X. 9</t>
-  </si>
-  <si>
     <t>Andree Prasetyo, S.Pd.</t>
   </si>
   <si>
@@ -232,9 +208,6 @@
     <t>19</t>
   </si>
   <si>
-    <t>X. 10</t>
-  </si>
-  <si>
     <t>Indah Sulmayanti, M.Pd.</t>
   </si>
   <si>
@@ -253,9 +226,6 @@
     <t>21</t>
   </si>
   <si>
-    <t>X. 11</t>
-  </si>
-  <si>
     <t>Pandu Aditya, M.Pd.</t>
   </si>
   <si>
@@ -274,9 +244,6 @@
     <t>23</t>
   </si>
   <si>
-    <t>XI. 1</t>
-  </si>
-  <si>
     <t>Try Puri anggraini, S.Pd., M.Pd.</t>
   </si>
   <si>
@@ -295,9 +262,6 @@
     <t>25</t>
   </si>
   <si>
-    <t>XI. 2</t>
-  </si>
-  <si>
     <t>Hermanto, S.Pd., M.Pd.</t>
   </si>
   <si>
@@ -316,9 +280,6 @@
     <t>27</t>
   </si>
   <si>
-    <t>XI. 3</t>
-  </si>
-  <si>
     <t>Nengsi Juita, M.Pd.Si.</t>
   </si>
   <si>
@@ -337,9 +298,6 @@
     <t>29</t>
   </si>
   <si>
-    <t>XI. 4</t>
-  </si>
-  <si>
     <t>Anggun Saymona, S.Pd., M.Pd.</t>
   </si>
   <si>
@@ -358,9 +316,6 @@
     <t>31</t>
   </si>
   <si>
-    <t>XI. 5</t>
-  </si>
-  <si>
     <t>Nyoman Kopariyanto, S.Pd.</t>
   </si>
   <si>
@@ -379,9 +334,6 @@
     <t>33</t>
   </si>
   <si>
-    <t>XI. 6</t>
-  </si>
-  <si>
     <t>Abdul Hafiz, S.Pd.</t>
   </si>
   <si>
@@ -400,9 +352,6 @@
     <t>35</t>
   </si>
   <si>
-    <t>XI. 7</t>
-  </si>
-  <si>
     <t>Singgih Sudarmawan, S.Ag.</t>
   </si>
   <si>
@@ -421,9 +370,6 @@
     <t>37</t>
   </si>
   <si>
-    <t>XI. 8</t>
-  </si>
-  <si>
     <t>Wely Marisa, S.Pd.</t>
   </si>
   <si>
@@ -433,9 +379,6 @@
     <t>38</t>
   </si>
   <si>
-    <t>XI. 9</t>
-  </si>
-  <si>
     <t>A.Thoriq Ganda, S.Pd.</t>
   </si>
   <si>
@@ -445,9 +388,6 @@
     <t>39</t>
   </si>
   <si>
-    <t>XI. 10</t>
-  </si>
-  <si>
     <t>Ari Yani A M, S.T.</t>
   </si>
   <si>
@@ -457,9 +397,6 @@
     <t>40</t>
   </si>
   <si>
-    <t>XI. 11</t>
-  </si>
-  <si>
     <t>Bagus Panca Wiratama, S.Pd., M.Pd.</t>
   </si>
   <si>
@@ -469,9 +406,6 @@
     <t>41</t>
   </si>
   <si>
-    <t>XII. 1</t>
-  </si>
-  <si>
     <t>Tri Tamti Nugraheni, S.Pd.</t>
   </si>
   <si>
@@ -490,9 +424,6 @@
     <t>43</t>
   </si>
   <si>
-    <t>XII. 2</t>
-  </si>
-  <si>
     <t>Titin Sumarni, S.Pd.</t>
   </si>
   <si>
@@ -511,9 +442,6 @@
     <t>45</t>
   </si>
   <si>
-    <t>XII. 3</t>
-  </si>
-  <si>
     <t>Nur Azizah, S.Pd.I.</t>
   </si>
   <si>
@@ -532,9 +460,6 @@
     <t>47</t>
   </si>
   <si>
-    <t>XII. 4</t>
-  </si>
-  <si>
     <t>Atik Apriliawati, S.Pd.</t>
   </si>
   <si>
@@ -553,9 +478,6 @@
     <t>49</t>
   </si>
   <si>
-    <t>XII. 5</t>
-  </si>
-  <si>
     <t>Nur Rohmad Safarudin, M.Pd.</t>
   </si>
   <si>
@@ -574,9 +496,6 @@
     <t>51</t>
   </si>
   <si>
-    <t>XII. 6</t>
-  </si>
-  <si>
     <t>Ade Ervani M, S.Sn.</t>
   </si>
   <si>
@@ -595,9 +514,6 @@
     <t>53</t>
   </si>
   <si>
-    <t>XII. 7</t>
-  </si>
-  <si>
     <t>Ribuwati, M.Pd.</t>
   </si>
   <si>
@@ -616,9 +532,6 @@
     <t>55</t>
   </si>
   <si>
-    <t>XII. 8</t>
-  </si>
-  <si>
     <t>Apriana, S.Pd.</t>
   </si>
   <si>
@@ -637,9 +550,6 @@
     <t>57</t>
   </si>
   <si>
-    <t>XII. 9</t>
-  </si>
-  <si>
     <t>Ari Astuti, S.Pd.</t>
   </si>
   <si>
@@ -658,9 +568,6 @@
     <t>59</t>
   </si>
   <si>
-    <t>XII. 10</t>
-  </si>
-  <si>
     <t>Muh. Zuhdi, S.Pd.</t>
   </si>
   <si>
@@ -674,13 +581,115 @@
   </si>
   <si>
     <t>fasil_ellys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AKUN FASILITATOR </t>
+  </si>
+  <si>
+    <t>KOKULIKULER SMAN 1 BELITANG 2026</t>
+  </si>
+  <si>
+    <t>X.1</t>
+  </si>
+  <si>
+    <t>X.2</t>
+  </si>
+  <si>
+    <t>X.3</t>
+  </si>
+  <si>
+    <t>X.4</t>
+  </si>
+  <si>
+    <t>X.5</t>
+  </si>
+  <si>
+    <t>X.6</t>
+  </si>
+  <si>
+    <t>X.7</t>
+  </si>
+  <si>
+    <t>X.8</t>
+  </si>
+  <si>
+    <t>X.9</t>
+  </si>
+  <si>
+    <t>X.10</t>
+  </si>
+  <si>
+    <t>X.11</t>
+  </si>
+  <si>
+    <t>XI.1</t>
+  </si>
+  <si>
+    <t>XI.2</t>
+  </si>
+  <si>
+    <t>XI.3</t>
+  </si>
+  <si>
+    <t>XI.4</t>
+  </si>
+  <si>
+    <t>XI.5</t>
+  </si>
+  <si>
+    <t>XI.6</t>
+  </si>
+  <si>
+    <t>XI.7</t>
+  </si>
+  <si>
+    <t>XI.8</t>
+  </si>
+  <si>
+    <t>XI.9</t>
+  </si>
+  <si>
+    <t>XI.10</t>
+  </si>
+  <si>
+    <t>XI.11</t>
+  </si>
+  <si>
+    <t>XII.1</t>
+  </si>
+  <si>
+    <t>XII.2</t>
+  </si>
+  <si>
+    <t>XII.3</t>
+  </si>
+  <si>
+    <t>XII.4</t>
+  </si>
+  <si>
+    <t>XII.5</t>
+  </si>
+  <si>
+    <t>XII.6</t>
+  </si>
+  <si>
+    <t>XII.7</t>
+  </si>
+  <si>
+    <t>XII.8</t>
+  </si>
+  <si>
+    <t>XII.9</t>
+  </si>
+  <si>
+    <t>XII.10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -693,16 +702,30 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -725,13 +748,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1036,1057 +1075,1083 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="B1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" customWidth="1"/>
+    <col min="2" max="2" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C5" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="C6" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C7" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="E7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="F7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C8" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="E8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="F8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C9" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="F9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C10" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C11" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="C12" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="E12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="C13" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B10" t="s">
+      <c r="E13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C14" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="E14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="F14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C15" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="E15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B12" t="s">
+      <c r="F15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C16" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="F16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="C17" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="F17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C18" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D14" t="s">
+      <c r="F18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="C19" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="E19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D15" t="s">
+      <c r="F19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="C20" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B16" t="s">
+      <c r="E20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C16" t="s">
+      <c r="F20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C21" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="E21" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="F21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C22" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="E22" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B18" t="s">
+      <c r="F22" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C23" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E23" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="F23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="C24" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E24" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="F24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C25" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E25" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D20" t="s">
+      <c r="F25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="C26" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="E26" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F26" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="C27" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B22" t="s">
+      <c r="E27" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C22" t="s">
+      <c r="F27" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C28" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="E28" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="F28" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D23" t="s">
+      <c r="C29" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="E29" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B24" t="s">
+      <c r="F29" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C30" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E30" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="F30" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B25" t="s">
-        <v>84</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="C31" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E31" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="F31" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B32" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C32" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E32" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F32" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="C33" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B27" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="E33" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D27" t="s">
+      <c r="F33" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B34" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="C34" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B28" t="s">
+      <c r="E34" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C28" t="s">
+      <c r="F34" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D28" t="s">
+      <c r="C35" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="E35" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B29" t="s">
-        <v>98</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="F35" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D29" t="s">
+      <c r="C36" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="E36" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B30" t="s">
+      <c r="F36" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B37" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C37" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E37" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="F37" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B31" t="s">
-        <v>105</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="C38" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E38" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E31" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="F38" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B39" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C39" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C32" t="s">
+      <c r="E39" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D32" t="s">
+      <c r="F39" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B40" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="C40" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B33" t="s">
-        <v>112</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="E40" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D33" t="s">
+      <c r="F40" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B41" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="C41" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B34" t="s">
+      <c r="E41" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C34" t="s">
+      <c r="F41" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B42" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D34" t="s">
+      <c r="C42" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E34" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="E42" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B35" t="s">
-        <v>119</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="F42" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B43" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D35" t="s">
+      <c r="C43" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="E43" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B36" t="s">
+      <c r="F43" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B44" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C44" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E44" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E36" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="F44" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B45" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B37" t="s">
-        <v>126</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="C45" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E45" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E37" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="F45" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B46" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C46" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C38" t="s">
+      <c r="E46" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D38" t="s">
+      <c r="F46" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B47" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E38" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="C47" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B39" t="s">
+      <c r="E47" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C39" t="s">
+      <c r="F47" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B48" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D39" t="s">
+      <c r="C48" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E39" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="E48" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B40" t="s">
+      <c r="F48" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B49" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C49" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E49" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E40" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="F49" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B50" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C50" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C41" t="s">
+      <c r="E50" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D41" t="s">
+      <c r="F50" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B51" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E41" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="C51" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B42" t="s">
+      <c r="E51" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C42" t="s">
+      <c r="F51" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B52" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D42" t="s">
+      <c r="C52" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E42" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="E52" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B43" t="s">
-        <v>149</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="F52" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B53" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D43" t="s">
+      <c r="C53" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E43" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="E53" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B44" t="s">
+      <c r="F53" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B54" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C54" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E54" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E44" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="F54" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B55" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B45" t="s">
-        <v>156</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="C55" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E55" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E45" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="F55" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B56" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C56" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C46" t="s">
+      <c r="E56" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D46" t="s">
+      <c r="F56" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B57" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E46" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="C57" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B47" t="s">
-        <v>163</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="E57" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D47" t="s">
+      <c r="F57" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B58" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E47" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="C58" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B48" t="s">
+      <c r="E58" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C48" t="s">
+      <c r="F58" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B59" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D48" t="s">
+      <c r="C59" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E48" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="E59" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B49" t="s">
-        <v>170</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="F59" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B60" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D49" t="s">
+      <c r="C60" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E49" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="E60" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B50" t="s">
+      <c r="F60" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B61" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C61" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E61" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E50" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="F61" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B62" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B51" t="s">
-        <v>177</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="C62" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E62" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E51" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="F62" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B63" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C63" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C52" t="s">
+      <c r="E63" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D52" t="s">
-        <v>186</v>
-      </c>
-      <c r="E52" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>187</v>
-      </c>
-      <c r="B53" t="s">
-        <v>184</v>
-      </c>
-      <c r="C53" t="s">
-        <v>188</v>
-      </c>
-      <c r="D53" t="s">
-        <v>189</v>
-      </c>
-      <c r="E53" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>190</v>
-      </c>
-      <c r="B54" t="s">
-        <v>191</v>
-      </c>
-      <c r="C54" t="s">
-        <v>192</v>
-      </c>
-      <c r="D54" t="s">
-        <v>193</v>
-      </c>
-      <c r="E54" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>194</v>
-      </c>
-      <c r="B55" t="s">
-        <v>191</v>
-      </c>
-      <c r="C55" t="s">
-        <v>195</v>
-      </c>
-      <c r="D55" t="s">
-        <v>196</v>
-      </c>
-      <c r="E55" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>197</v>
-      </c>
-      <c r="B56" t="s">
-        <v>198</v>
-      </c>
-      <c r="C56" t="s">
-        <v>199</v>
-      </c>
-      <c r="D56" t="s">
-        <v>200</v>
-      </c>
-      <c r="E56" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>201</v>
-      </c>
-      <c r="B57" t="s">
-        <v>198</v>
-      </c>
-      <c r="C57" t="s">
-        <v>202</v>
-      </c>
-      <c r="D57" t="s">
-        <v>203</v>
-      </c>
-      <c r="E57" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>204</v>
-      </c>
-      <c r="B58" t="s">
-        <v>205</v>
-      </c>
-      <c r="C58" t="s">
-        <v>206</v>
-      </c>
-      <c r="D58" t="s">
-        <v>207</v>
-      </c>
-      <c r="E58" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>208</v>
-      </c>
-      <c r="B59" t="s">
-        <v>205</v>
-      </c>
-      <c r="C59" t="s">
-        <v>209</v>
-      </c>
-      <c r="D59" t="s">
-        <v>210</v>
-      </c>
-      <c r="E59" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>211</v>
-      </c>
-      <c r="B60" t="s">
-        <v>212</v>
-      </c>
-      <c r="C60" t="s">
-        <v>213</v>
-      </c>
-      <c r="D60" t="s">
-        <v>214</v>
-      </c>
-      <c r="E60" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>215</v>
-      </c>
-      <c r="B61" t="s">
-        <v>212</v>
-      </c>
-      <c r="C61" t="s">
-        <v>216</v>
-      </c>
-      <c r="D61" t="s">
-        <v>217</v>
-      </c>
-      <c r="E61" t="s">
-        <v>9</v>
+      <c r="F63" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <mergeCells count="2">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+  </mergeCells>
+  <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: improve student material dashboard UI - navigation pills, Bagian titles, and icon size fixes
</commit_message>
<xml_diff>
--- a/Akun_Fasilitator_Kokulikuler.xlsx
+++ b/Akun_Fasilitator_Kokulikuler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aplikasi Web AI\LP Kokulikuler SMAN 1 Belitang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB5E5A9-8D36-4E33-A4FA-9F7D05114F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAA50E2-204B-472C-BB38-A905BFC28595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -689,7 +689,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -706,6 +706,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -758,10 +766,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -773,8 +782,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1078,7 +1089,7 @@
   <dimension ref="B1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1870,7 +1881,7 @@
       <c r="E47" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F47" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1887,7 +1898,7 @@
       <c r="E48" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="F48" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2151,7 +2162,11 @@
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F48" r:id="rId1" xr:uid="{F93CE807-E8B3-4C0F-8782-90B08EE69E93}"/>
+    <hyperlink ref="F47" r:id="rId2" xr:uid="{993AE395-958F-4C9D-AF7B-EDB2B040E325}"/>
+  </hyperlinks>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>